<commit_message>
FE, BE实装Token but not tested
</commit_message>
<xml_diff>
--- a/Document/詳細設計書/Table定義書.xlsx
+++ b/Document/詳細設計書/Table定義書.xlsx
@@ -1,22 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24026"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/945ad830e40d5886/文档/2021春季毕设文件夹/Documents/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Git\CourseManagementSystem-1\Document\詳細設計書\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="63" documentId="11_AD4DA82427541F7ACA7EB8D2A08F0E386AE8DE14" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{5515B76F-DE49-4E9E-A6EC-17712C0256CC}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F73909BD-1036-47CE-98D3-D3B0E94675C6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1185" yWindow="1875" windowWidth="24825" windowHeight="11955" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-225" yWindow="1725" windowWidth="21600" windowHeight="11505" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Index" sheetId="1" r:id="rId1"/>
     <sheet name="admin" sheetId="3" r:id="rId2"/>
     <sheet name="student" sheetId="4" r:id="rId3"/>
     <sheet name="Template" sheetId="2" r:id="rId4"/>
+    <sheet name="token" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -28,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="34">
   <si>
     <t>No.</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -139,6 +140,30 @@
   </si>
   <si>
     <t>未确定，应是定长Hash</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>token</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>varchar()</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Token</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>role</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>连接其他表</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>连接表名</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -942,8 +967,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{822FAC8C-2742-4BF2-91D2-F30B1C9E787D}">
   <dimension ref="A1:J12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K19" sqref="K19"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -1089,4 +1114,188 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6428C651-B23C-485A-9308-AECF5D8590D4}">
+  <dimension ref="A1:J12"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="M8" sqref="M8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="2" width="9" style="1"/>
+    <col min="3" max="3" width="13.125" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.125" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9" style="1"/>
+    <col min="6" max="7" width="11.125" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.875" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="8.25" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="11.125" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="12.875" style="1" bestFit="1" customWidth="1"/>
+    <col min="12" max="16384" width="9" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" s="9" customFormat="1" ht="18" x14ac:dyDescent="0.25">
+      <c r="A1" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="C1" s="8"/>
+    </row>
+    <row r="3" spans="1:10" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="B4" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="D4" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="E4" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="F4" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="G4" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="H4" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="I4" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="J4" s="5" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="B5" s="7">
+        <v>0</v>
+      </c>
+      <c r="C5" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="D5" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="E5" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="F5" s="7">
+        <v>1</v>
+      </c>
+      <c r="G5" s="7"/>
+      <c r="H5" s="7"/>
+      <c r="I5" s="7">
+        <v>1</v>
+      </c>
+      <c r="J5" s="7"/>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="B6" s="7">
+        <v>1</v>
+      </c>
+      <c r="C6" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="D6" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="E6" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="F6" s="7"/>
+      <c r="G6" s="7"/>
+      <c r="H6" s="7"/>
+      <c r="I6" s="7">
+        <v>1</v>
+      </c>
+      <c r="J6" s="7"/>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="B7" s="7">
+        <v>2</v>
+      </c>
+      <c r="C7" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="D7" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="E7" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="F7" s="7"/>
+      <c r="G7" s="7"/>
+      <c r="H7" s="7"/>
+      <c r="I7" s="7">
+        <v>1</v>
+      </c>
+      <c r="J7" s="7"/>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="B8" s="7"/>
+      <c r="C8" s="7"/>
+      <c r="D8" s="7"/>
+      <c r="E8" s="7"/>
+      <c r="F8" s="7"/>
+      <c r="G8" s="7"/>
+      <c r="H8" s="7"/>
+      <c r="I8" s="7"/>
+      <c r="J8" s="7"/>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="B9" s="7"/>
+      <c r="C9" s="7"/>
+      <c r="D9" s="7"/>
+      <c r="E9" s="7"/>
+      <c r="F9" s="7"/>
+      <c r="G9" s="7"/>
+      <c r="H9" s="7"/>
+      <c r="I9" s="7"/>
+      <c r="J9" s="7"/>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="B10" s="7"/>
+      <c r="C10" s="7"/>
+      <c r="D10" s="7"/>
+      <c r="E10" s="7"/>
+      <c r="F10" s="7"/>
+      <c r="G10" s="7"/>
+      <c r="H10" s="7"/>
+      <c r="I10" s="7"/>
+      <c r="J10" s="7"/>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="B11" s="7"/>
+      <c r="C11" s="7"/>
+      <c r="D11" s="7"/>
+      <c r="E11" s="7"/>
+      <c r="F11" s="7"/>
+      <c r="G11" s="7"/>
+      <c r="H11" s="7"/>
+      <c r="I11" s="7"/>
+      <c r="J11" s="7"/>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="B12" s="7"/>
+      <c r="C12" s="7"/>
+      <c r="D12" s="7"/>
+      <c r="E12" s="7"/>
+      <c r="F12" s="7"/>
+      <c r="G12" s="7"/>
+      <c r="H12" s="7"/>
+      <c r="I12" s="7"/>
+      <c r="J12" s="7"/>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>